<commit_message>
Fix minor error in actual_lineups
</commit_message>
<xml_diff>
--- a/actual_lineups.xlsx
+++ b/actual_lineups.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashha\Desktop\my files\MIT\coursework\Fall 2022\6.255\Optimization-Final-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mohammedahmed/Dropbox (Personal)/Mac/Desktop/6.7201/Optimization-Final-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348148AD-7B36-45AA-98B2-C6B183F16F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B548771-2CD9-2944-9397-5648AD360302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" firstSheet="37" activeTab="37" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="6380" yWindow="500" windowWidth="24800" windowHeight="16860" firstSheet="13" activeTab="15" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Norwich City_1" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>cf</t>
   </si>
   <si>
-    <t>I. KonatÃ©</t>
-  </si>
-  <si>
     <t>C. Jones</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>T. Minamino</t>
+  </si>
+  <si>
+    <t>I. Konaté</t>
   </si>
 </sst>
 </file>
@@ -542,9 +542,9 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -552,7 +552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -560,7 +560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -568,7 +568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -576,7 +576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -584,7 +584,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -592,7 +592,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -600,7 +600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -608,7 +608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -624,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -632,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>23</v>
       </c>
@@ -650,9 +650,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -660,7 +660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -668,15 +668,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -684,7 +684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -692,7 +692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -700,7 +700,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -708,15 +708,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -732,7 +732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -750,12 +750,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -763,7 +763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -771,7 +771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -779,7 +779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -787,7 +787,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -795,7 +795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -803,7 +803,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -811,7 +811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -819,7 +819,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -835,7 +835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -856,9 +856,9 @@
       <selection activeCell="A8" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -866,7 +866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -874,7 +874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -882,7 +882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -890,7 +890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -898,7 +898,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -906,7 +906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -914,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -930,7 +930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -938,7 +938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -959,9 +959,9 @@
       <selection activeCell="A9" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -969,7 +969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -977,15 +977,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -993,7 +993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1062,9 +1062,9 @@
       <selection activeCell="A6" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1165,9 +1165,9 @@
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1264,13 +1264,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499942B5-2A2C-4BCE-954D-5192B70EFA96}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1278,7 +1278,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1368,12 +1368,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:B11"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1381,15 +1381,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1474,9 +1474,9 @@
       <selection activeCell="A7" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1484,15 +1484,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1516,15 +1516,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1577,9 +1577,9 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1587,15 +1587,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1619,7 +1619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1635,15 +1635,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1651,17 +1651,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1680,9 +1680,9 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1780,12 +1780,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:B11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1793,15 +1793,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1833,7 +1833,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1886,33 +1886,33 @@
       <selection activeCell="A9" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1989,9 +1989,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1999,15 +1999,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2047,15 +2047,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2063,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2092,9 +2092,9 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2102,15 +2102,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2150,15 +2150,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2195,9 +2195,9 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2205,15 +2205,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2245,7 +2245,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2253,15 +2253,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2269,15 +2269,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2298,9 +2298,9 @@
       <selection activeCell="A11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2308,15 +2308,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2372,15 +2372,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2401,9 +2401,9 @@
       <selection activeCell="A8" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2411,15 +2411,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2475,17 +2475,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2504,9 +2504,9 @@
       <selection activeCell="A11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2514,15 +2514,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2570,23 +2570,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -2607,9 +2607,9 @@
       <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2617,23 +2617,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2681,17 +2681,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2710,9 +2710,9 @@
       <selection activeCell="A10" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2720,15 +2720,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2784,17 +2784,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2813,9 +2813,9 @@
       <selection activeCell="B11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2916,9 +2916,9 @@
       <selection activeCell="A11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -2926,15 +2926,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2990,17 +2990,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -3019,9 +3019,9 @@
       <selection activeCell="A11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3029,15 +3029,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3077,15 +3077,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3093,7 +3093,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3122,9 +3122,9 @@
       <selection activeCell="B10" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3132,15 +3132,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3196,15 +3196,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3225,9 +3225,9 @@
       <selection activeCell="A9" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3235,15 +3235,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3275,7 +3275,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -3283,23 +3283,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3307,9 +3307,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -3328,9 +3328,9 @@
       <selection activeCell="A11" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3338,15 +3338,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3402,15 +3402,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3431,9 +3431,9 @@
       <selection activeCell="A10" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3441,15 +3441,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3497,23 +3497,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3534,9 +3534,9 @@
       <selection activeCell="A10" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3544,23 +3544,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -3608,17 +3608,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -3637,9 +3637,9 @@
       <selection activeCell="B10" sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3655,15 +3655,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3695,23 +3695,23 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -3736,13 +3736,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7509E4AC-9A11-4F64-B623-0071E271D58A}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -3758,15 +3758,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -3790,7 +3790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3814,17 +3814,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -3843,9 +3843,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -3869,7 +3869,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -3943,12 +3943,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3972,15 +3972,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4049,9 +4049,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4059,7 +4059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4075,7 +4075,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4099,15 +4099,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4152,9 +4152,9 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4194,7 +4194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4202,15 +4202,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -4252,20 +4252,20 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:B11"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -4281,7 +4281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4305,7 +4305,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -4313,7 +4313,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4337,9 +4337,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -4358,9 +4358,9 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4376,15 +4376,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -4440,9 +4440,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>

</xml_diff>